<commit_message>
Da Mystery of da Chesswhale
TIGER STYLE
</commit_message>
<xml_diff>
--- a/data/strings/zoneData.xlsx
+++ b/data/strings/zoneData.xlsx
@@ -134,9 +134,6 @@
     <t xml:space="preserve"> The digital world is a wonderful world, but at some point you will need to work with real life as well. Physical design helps you taking your project from a sketch to the real world.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Greetings young one, and welcome to Medialogy. To begin your quest, place your finger on top of your avatar and drag yourself through the path of Medialogy.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Once you understand the digital and the physical world, it’s time to make the real magic: Animation._You dont need to be Disney or Pixar to make things move, and already on first semester you will be animating.</t>
   </si>
   <si>
@@ -150,6 +147,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Shapes, sprites and polygons. The world of computer graphics will always be closely related to programming. To make your ideas work in real life, you will work with the tools necessary to make 2D and 3D graphics.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Greetings young one, and welcome to Medialogy,  a bachelor and masters degree at Aalborg University _To begin your quest, place your finger on top of your avatar and drag yourself through the path of Medialogy.</t>
   </si>
 </sst>
 </file>
@@ -504,7 +504,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -530,7 +530,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
         <v>33</v>
@@ -544,7 +544,7 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -563,10 +563,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -596,10 +596,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>